<commit_message>
new NC data and text
</commit_message>
<xml_diff>
--- a/data/source/JRI infographic data.xlsx
+++ b/data/source/JRI infographic data.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -277,10 +280,27 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -303,17 +323,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -328,39 +366,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,201 +477,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -641,11 +620,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:53">
       <c r="A1" t="s">
@@ -2116,25 +2105,25 @@
         <v>43220</v>
       </c>
       <c r="AA13">
-        <v>2067</v>
+        <v>2262</v>
       </c>
       <c r="AB13">
-        <v>2061</v>
+        <v>2268</v>
       </c>
       <c r="AC13">
-        <v>1900</v>
+        <v>2358</v>
       </c>
       <c r="AD13">
-        <v>1829</v>
+        <v>2793</v>
       </c>
       <c r="AE13">
-        <v>1612</v>
+        <v>4970</v>
       </c>
       <c r="AF13">
-        <v>1467</v>
+        <v>7913</v>
       </c>
       <c r="AG13">
-        <v>1407</v>
+        <v>10355</v>
       </c>
       <c r="AJ13">
         <v>109540</v>
@@ -2557,49 +2546,61 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:53">
+    <row r="17" spans="1:53" s="4" customFormat="1">
       <c r="A17" t="s">
         <v>77</v>
       </c>
-      <c r="D17">
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17" s="1">
         <v>50622</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>51281</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>51290</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>51757</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>51382</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>51118</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>50366</v>
       </c>
-      <c r="O17">
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17" s="1">
         <v>51638</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="1">
         <v>51722</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="1">
         <v>52279</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="1">
         <v>52236</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="1">
         <v>51693</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="1">
         <v>51151</v>
       </c>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
       <c r="AA17">
         <v>23224</v>
       </c>
@@ -2621,6 +2622,8 @@
       <c r="AG17">
         <v>33076</v>
       </c>
+      <c r="AH17"/>
+      <c r="AI17"/>
       <c r="AJ17">
         <v>7876</v>
       </c>
@@ -2654,7 +2657,7 @@
       <c r="AT17">
         <v>2011</v>
       </c>
-      <c r="AU17" t="s">
+      <c r="AU17" s="2" t="s">
         <v>55</v>
       </c>
       <c r="AV17">
@@ -2663,13 +2666,13 @@
       <c r="AW17">
         <v>2015</v>
       </c>
-      <c r="AX17" t="s">
+      <c r="AX17" s="3" t="s">
         <v>78</v>
       </c>
       <c r="AY17">
         <v>2015</v>
       </c>
-      <c r="AZ17" t="s">
+      <c r="AZ17" s="3" t="s">
         <v>78</v>
       </c>
       <c r="BA17">
@@ -3013,7 +3016,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
correct col header in data
</commit_message>
<xml_diff>
--- a/data/source/JRI infographic data.xlsx
+++ b/data/source/JRI infographic data.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13275" yWindow="15" windowWidth="15525" windowHeight="12810"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
   <si>
     <t>State</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>West Virginia</t>
+  </si>
+  <si>
+    <t>PROJ_2020</t>
   </si>
 </sst>
 </file>
@@ -275,18 +278,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -321,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -330,22 +333,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -360,39 +354,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,7 +421,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,142 +465,201 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -614,26 +667,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" customWidth="1"/>
-    <col min="37" max="40" width="10" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -704,7 +744,7 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="Y1" t="s">
         <v>23</v>
@@ -794,7 +834,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -919,7 +959,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -996,7 +1036,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1115,7 +1155,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1234,7 +1274,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1356,7 +1396,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1478,7 +1518,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1585,7 +1625,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1698,7 +1738,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1805,7 +1845,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1930,7 +1970,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -2052,7 +2092,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -2177,7 +2217,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2308,7 +2348,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2433,7 +2473,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2543,12 +2583,10 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53">
       <c r="A17" t="s">
         <v>77</v>
       </c>
-      <c r="B17"/>
-      <c r="C17"/>
       <c r="D17" s="1">
         <v>50622</v>
       </c>
@@ -2570,10 +2608,6 @@
       <c r="J17" s="1">
         <v>50366</v>
       </c>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="N17"/>
       <c r="O17" s="1">
         <v>51638</v>
       </c>
@@ -2592,12 +2626,6 @@
       <c r="T17" s="1">
         <v>51151</v>
       </c>
-      <c r="U17"/>
-      <c r="V17"/>
-      <c r="W17"/>
-      <c r="X17"/>
-      <c r="Y17"/>
-      <c r="Z17"/>
       <c r="AA17">
         <v>23224</v>
       </c>
@@ -2619,8 +2647,6 @@
       <c r="AG17">
         <v>33076</v>
       </c>
-      <c r="AH17"/>
-      <c r="AI17"/>
       <c r="AJ17">
         <v>7876</v>
       </c>
@@ -2676,7 +2702,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -2801,7 +2827,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2917,7 +2943,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -3013,6 +3039,11 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
copy edited text and new data
</commit_message>
<xml_diff>
--- a/data/source/JRI infographic data.xlsx
+++ b/data/source/JRI infographic data.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/jri/data/source/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="12140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t>State</t>
   </si>
@@ -271,6 +282,9 @@
   </si>
   <si>
     <t>On an average day in fiscal year</t>
+  </si>
+  <si>
+    <t>PROJ_2020</t>
   </si>
 </sst>
 </file>
@@ -607,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -617,25 +631,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomRight" activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.5" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="17" customWidth="1"/>
-    <col min="51" max="51" width="11.42578125" customWidth="1"/>
-    <col min="52" max="52" width="17.85546875" customWidth="1"/>
+    <col min="51" max="51" width="11.5" customWidth="1"/>
+    <col min="52" max="52" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +720,7 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="Y1" t="s">
         <v>23</v>
@@ -796,7 +810,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -927,7 +941,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1004,7 +1018,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1123,7 +1137,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1242,7 +1256,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1364,7 +1378,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1486,7 +1500,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1605,7 +1619,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1724,7 +1738,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1831,7 +1845,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1956,7 +1970,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -2078,7 +2092,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -2203,7 +2217,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2334,7 +2348,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2459,7 +2473,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2569,7 +2583,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -2702,7 +2716,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -2794,7 +2808,7 @@
         <v>26809</v>
       </c>
       <c r="AQ18">
-        <v>24891463</v>
+        <v>341891463</v>
       </c>
       <c r="AR18">
         <v>0</v>
@@ -2827,7 +2841,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2943,7 +2957,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
final final final final final final text
</commit_message>
<xml_diff>
--- a/data/source/JRI infographic data.xlsx
+++ b/data/source/JRI infographic data.xlsx
@@ -1,28 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/jri/data/source/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="12140"/>
+    <workbookView xWindow="14100" yWindow="-45" windowWidth="14505" windowHeight="12825"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -621,7 +610,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -631,25 +620,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X2" sqref="X2"/>
+      <selection pane="bottomRight" activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="17" customWidth="1"/>
-    <col min="51" max="51" width="11.5" customWidth="1"/>
-    <col min="52" max="52" width="17.83203125" customWidth="1"/>
+    <col min="51" max="51" width="11.42578125" customWidth="1"/>
+    <col min="52" max="52" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -810,7 +801,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -941,7 +932,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1018,7 +1009,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1137,7 +1128,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1153,11 +1144,11 @@
       <c r="G5">
         <v>6060</v>
       </c>
-      <c r="H5">
-        <v>5643</v>
-      </c>
-      <c r="I5">
-        <v>5993</v>
+      <c r="H5" s="4">
+        <v>5853</v>
+      </c>
+      <c r="I5" s="4">
+        <v>5819</v>
       </c>
       <c r="J5">
         <v>6024</v>
@@ -1256,7 +1247,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1324,13 +1315,13 @@
         <v>3416</v>
       </c>
       <c r="AJ6">
+        <v>10164</v>
+      </c>
+      <c r="AK6">
         <v>10048</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>10097</v>
-      </c>
-      <c r="AL6">
-        <v>10239</v>
       </c>
       <c r="AM6">
         <v>10096</v>
@@ -1339,10 +1330,10 @@
         <v>10239</v>
       </c>
       <c r="AO6">
+        <v>10680</v>
+      </c>
+      <c r="AP6">
         <v>10755</v>
-      </c>
-      <c r="AP6">
-        <v>11155</v>
       </c>
       <c r="AQ6">
         <v>17725165</v>
@@ -1378,7 +1369,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1434,16 +1425,16 @@
         <v>5938</v>
       </c>
       <c r="AD7">
-        <v>5848</v>
+        <v>5845</v>
       </c>
       <c r="AE7">
         <v>5593</v>
       </c>
       <c r="AF7">
-        <v>4725</v>
+        <v>4723</v>
       </c>
       <c r="AG7">
-        <v>4808</v>
+        <v>4804</v>
       </c>
       <c r="AJ7">
         <v>8011</v>
@@ -1500,7 +1491,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -1619,7 +1610,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1738,7 +1729,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1845,7 +1836,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1970,7 +1961,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -2092,7 +2083,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>71</v>
       </c>
@@ -2121,7 +2112,7 @@
         <v>37794</v>
       </c>
       <c r="O13">
-        <v>41130</v>
+        <v>41811</v>
       </c>
       <c r="P13">
         <v>41987</v>
@@ -2141,26 +2132,35 @@
       <c r="U13">
         <v>43220</v>
       </c>
+      <c r="V13">
+        <v>43664</v>
+      </c>
+      <c r="W13">
+        <v>44208</v>
+      </c>
+      <c r="X13">
+        <v>44840</v>
+      </c>
       <c r="AA13">
-        <v>2262</v>
+        <v>4329</v>
       </c>
       <c r="AB13">
-        <v>2268</v>
+        <v>4329</v>
       </c>
       <c r="AC13">
-        <v>2358</v>
+        <v>4258</v>
       </c>
       <c r="AD13">
-        <v>2793</v>
+        <v>4622</v>
       </c>
       <c r="AE13">
-        <v>4970</v>
+        <v>6582</v>
       </c>
       <c r="AF13">
-        <v>7913</v>
+        <v>9380</v>
       </c>
       <c r="AG13">
-        <v>10355</v>
+        <v>11762</v>
       </c>
       <c r="AJ13">
         <v>109540</v>
@@ -2217,7 +2217,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2246,31 +2246,22 @@
         <v>50651</v>
       </c>
       <c r="N14">
-        <v>51722</v>
+        <v>50987</v>
       </c>
       <c r="O14">
-        <v>52546</v>
+        <v>51297</v>
       </c>
       <c r="P14">
-        <v>53176</v>
+        <v>52164</v>
       </c>
       <c r="Q14">
-        <v>53926</v>
+        <v>52784</v>
       </c>
       <c r="R14">
-        <v>54429</v>
+        <v>53413</v>
       </c>
       <c r="S14">
-        <v>54804</v>
-      </c>
-      <c r="T14">
-        <v>55342</v>
-      </c>
-      <c r="U14">
-        <v>55560</v>
-      </c>
-      <c r="V14">
-        <v>55734</v>
+        <v>53858</v>
       </c>
       <c r="AA14">
         <v>13637</v>
@@ -2348,7 +2339,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2371,31 +2362,7 @@
         <v>28182</v>
       </c>
       <c r="J15">
-        <v>28095</v>
-      </c>
-      <c r="O15">
-        <v>26692</v>
-      </c>
-      <c r="P15">
-        <v>27159</v>
-      </c>
-      <c r="Q15">
-        <v>27569</v>
-      </c>
-      <c r="R15">
-        <v>27887</v>
-      </c>
-      <c r="S15">
-        <v>28232</v>
-      </c>
-      <c r="T15">
-        <v>28534</v>
-      </c>
-      <c r="U15">
-        <v>28798</v>
-      </c>
-      <c r="V15">
-        <v>29072</v>
+        <v>28871</v>
       </c>
       <c r="AA15">
         <v>3706</v>
@@ -2416,7 +2383,7 @@
         <v>3204</v>
       </c>
       <c r="AG15">
-        <v>2764</v>
+        <v>2981</v>
       </c>
       <c r="AJ15">
         <v>27464</v>
@@ -2437,7 +2404,7 @@
         <v>21586</v>
       </c>
       <c r="AP15">
-        <v>23658</v>
+        <v>22957</v>
       </c>
       <c r="AQ15">
         <v>0</v>
@@ -2473,7 +2440,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2583,7 +2550,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -2716,7 +2683,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -2808,7 +2775,7 @@
         <v>26809</v>
       </c>
       <c r="AQ18">
-        <v>341891463</v>
+        <v>491000000</v>
       </c>
       <c r="AR18">
         <v>0</v>
@@ -2841,7 +2808,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -2957,7 +2924,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
updated with 2016 data
</commit_message>
<xml_diff>
--- a/data/source/JRI infographic data.xlsx
+++ b/data/source/JRI infographic data.xlsx
@@ -1,17 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/jri/data/source/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12195" yWindow="45" windowWidth="12015" windowHeight="12780"/>
+    <workbookView xWindow="4580" yWindow="760" windowWidth="21400" windowHeight="19880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="89">
   <si>
     <t>State</t>
   </si>
@@ -192,9 +203,6 @@
     <t>On December 31st,</t>
   </si>
   <si>
-    <t>In December,</t>
-  </si>
-  <si>
     <t>Hawaii</t>
   </si>
   <si>
@@ -277,6 +285,18 @@
   </si>
   <si>
     <t>In July,</t>
+  </si>
+  <si>
+    <t>PRI_2016</t>
+  </si>
+  <si>
+    <t>PAR_2016</t>
+  </si>
+  <si>
+    <t>PRO_2016</t>
+  </si>
+  <si>
+    <t>In November,</t>
   </si>
 </sst>
 </file>
@@ -333,13 +353,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -613,7 +633,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -621,30 +641,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA20"/>
+  <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17" customWidth="1"/>
-    <col min="51" max="51" width="11.42578125" customWidth="1"/>
-    <col min="52" max="52" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="25" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10" customWidth="1"/>
+    <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17" style="3" customWidth="1"/>
+    <col min="54" max="54" width="11.5" customWidth="1"/>
+    <col min="55" max="55" width="17.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -676,136 +695,145 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
-        <v>83</v>
-      </c>
       <c r="Y1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AT1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -833,110 +861,119 @@
       <c r="J2">
         <v>17684</v>
       </c>
-      <c r="N2">
+      <c r="K2">
+        <v>17951</v>
+      </c>
+      <c r="O2">
         <v>15916</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>16767</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>17440</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>18147</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>18688</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>19222</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>19734</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>19974</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>21445</v>
       </c>
-      <c r="AB2">
+      <c r="AC2">
         <v>21774</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>23407</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>23657</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>22721</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>22414</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>21708</v>
       </c>
       <c r="AI2">
+        <v>23518</v>
+      </c>
+      <c r="AK2">
         <v>30997</v>
       </c>
-      <c r="AJ2">
+      <c r="AL2">
         <v>29793</v>
       </c>
-      <c r="AK2">
+      <c r="AM2">
         <v>28156</v>
       </c>
-      <c r="AL2">
+      <c r="AN2">
         <v>29741</v>
       </c>
-      <c r="AM2">
+      <c r="AO2">
         <v>29528</v>
       </c>
-      <c r="AN2">
+      <c r="AP2">
         <v>28646</v>
       </c>
-      <c r="AO2">
+      <c r="AQ2">
         <v>27756</v>
       </c>
-      <c r="AP2">
+      <c r="AR2">
         <v>27127</v>
       </c>
-      <c r="AQ2">
+      <c r="AS2">
+        <v>30547</v>
+      </c>
+      <c r="AT2">
         <v>0</v>
       </c>
-      <c r="AR2">
+      <c r="AU2">
         <v>2400000</v>
       </c>
-      <c r="AS2">
+      <c r="AV2">
         <v>2011</v>
       </c>
-      <c r="AT2">
+      <c r="AW2">
         <v>2010</v>
       </c>
-      <c r="AU2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AV2">
+      <c r="AX2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY2">
+        <v>2016</v>
+      </c>
+      <c r="AZ2">
         <v>2015</v>
       </c>
-      <c r="AW2">
-        <v>2015</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="BA2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY2">
-        <v>2015</v>
-      </c>
-      <c r="AZ2" t="s">
+      <c r="BB2">
+        <v>2016</v>
+      </c>
+      <c r="BC2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA2">
-        <v>2015</v>
+      <c r="BD2">
+        <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -955,8 +992,8 @@
       <c r="J3">
         <v>6704</v>
       </c>
-      <c r="O3">
-        <v>6600</v>
+      <c r="K3">
+        <v>6432</v>
       </c>
       <c r="P3">
         <v>6600</v>
@@ -965,55 +1002,61 @@
         <v>6600</v>
       </c>
       <c r="R3">
+        <v>6600</v>
+      </c>
+      <c r="S3">
         <v>6650</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>6675</v>
       </c>
-      <c r="AL3">
+      <c r="AN3">
         <v>16523</v>
       </c>
-      <c r="AM3">
+      <c r="AO3">
         <v>16223</v>
       </c>
-      <c r="AN3">
+      <c r="AP3">
         <v>15995</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>16227</v>
       </c>
-      <c r="AP3">
+      <c r="AR3">
         <v>16089</v>
       </c>
-      <c r="AQ3">
+      <c r="AS3">
+        <v>15569</v>
+      </c>
+      <c r="AT3">
         <v>0</v>
       </c>
-      <c r="AR3">
+      <c r="AU3">
         <v>0</v>
       </c>
-      <c r="AS3">
+      <c r="AV3">
         <v>2012</v>
       </c>
-      <c r="AT3">
+      <c r="AW3">
         <v>2011</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AX3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AV3">
+      <c r="AY3">
+        <v>2016</v>
+      </c>
+      <c r="AZ3">
         <v>2015</v>
       </c>
-      <c r="AW3">
-        <v>2015</v>
-      </c>
-      <c r="AX3" t="s">
+      <c r="BA3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY3">
-        <v>2015</v>
+      <c r="BB3">
+        <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1038,100 +1081,109 @@
       <c r="J4">
         <v>53102</v>
       </c>
-      <c r="P4">
+      <c r="K4">
+        <v>54317</v>
+      </c>
+      <c r="Q4">
         <v>55933</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>56664</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>57492</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>58664</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>59553</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>59732</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <v>21307</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <v>22403</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>23729</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>22480</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>25020</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>25195</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>23859</v>
       </c>
-      <c r="AK4">
+      <c r="AI4">
+        <v>22901</v>
+      </c>
+      <c r="AM4">
         <v>156554</v>
       </c>
-      <c r="AL4">
+      <c r="AN4">
         <v>163709</v>
       </c>
-      <c r="AM4">
+      <c r="AO4">
         <v>163400</v>
       </c>
-      <c r="AN4">
+      <c r="AP4">
         <v>164484</v>
       </c>
-      <c r="AO4">
+      <c r="AQ4">
         <v>166207</v>
       </c>
-      <c r="AP4">
+      <c r="AR4">
         <v>167388</v>
       </c>
-      <c r="AQ4">
+      <c r="AS4">
+        <v>165635</v>
+      </c>
+      <c r="AT4">
         <v>264000000</v>
       </c>
-      <c r="AR4">
+      <c r="AU4">
         <v>56507694</v>
       </c>
-      <c r="AS4">
+      <c r="AV4">
         <v>2012</v>
       </c>
-      <c r="AT4">
+      <c r="AW4">
         <v>2011</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AX4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AV4">
+      <c r="AY4">
+        <v>2016</v>
+      </c>
+      <c r="AZ4">
         <v>2015</v>
       </c>
-      <c r="AW4">
-        <v>2015</v>
-      </c>
-      <c r="AX4" t="s">
+      <c r="BA4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="BB4">
+        <v>2016</v>
+      </c>
+      <c r="BC4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD4">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>57</v>
-      </c>
-      <c r="AY4">
-        <v>2015</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>54</v>
-      </c>
-      <c r="BA4">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>58</v>
       </c>
       <c r="D5">
         <v>6005</v>
@@ -1145,112 +1197,121 @@
       <c r="G5">
         <v>6060</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="2">
         <v>5853</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="2">
         <v>5819</v>
       </c>
       <c r="J5">
         <v>6024</v>
       </c>
-      <c r="P5">
+      <c r="K5">
+        <v>5970</v>
+      </c>
+      <c r="Q5">
         <v>6060</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>6132</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>6163</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>6193</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>6224</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>6255</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>6287</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <v>1869</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <v>1862</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>1839</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>1632</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>1589</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>1647</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>1545</v>
       </c>
-      <c r="AJ5">
+      <c r="AI5">
+        <v>1479</v>
+      </c>
+      <c r="AL5">
         <v>20586</v>
       </c>
-      <c r="AL5">
+      <c r="AN5">
         <v>23063</v>
       </c>
-      <c r="AM5">
+      <c r="AO5">
         <v>22654</v>
       </c>
-      <c r="AN5">
+      <c r="AP5">
         <v>21510</v>
       </c>
-      <c r="AO5">
+      <c r="AQ5">
         <v>20908</v>
       </c>
-      <c r="AP5">
+      <c r="AR5">
         <v>20828</v>
       </c>
-      <c r="AQ5">
+      <c r="AS5">
+        <v>20475</v>
+      </c>
+      <c r="AT5">
         <v>2500000</v>
       </c>
-      <c r="AR5">
+      <c r="AU5">
         <v>10600000</v>
       </c>
-      <c r="AS5">
+      <c r="AV5">
         <v>2012</v>
       </c>
-      <c r="AT5">
+      <c r="AW5">
         <v>2011</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AX5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY5">
+        <v>2016</v>
+      </c>
+      <c r="AZ5">
+        <v>2015</v>
+      </c>
+      <c r="BA5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BB5">
+        <v>2016</v>
+      </c>
+      <c r="BC5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD5">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>59</v>
-      </c>
-      <c r="AV5">
-        <v>2015</v>
-      </c>
-      <c r="AW5">
-        <v>2015</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AY5">
-        <v>2015</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>54</v>
-      </c>
-      <c r="BA5">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>60</v>
       </c>
       <c r="D6">
         <v>7283</v>
@@ -1273,106 +1334,115 @@
       <c r="J6">
         <v>8160</v>
       </c>
-      <c r="Q6">
+      <c r="K6">
+        <v>7713</v>
+      </c>
+      <c r="R6">
         <v>8160</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>8267</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>8506</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>8751</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>9001</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>9253</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>9408</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>2628</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <v>2847</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>2954</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>2883</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>2974</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>3056</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>3416</v>
       </c>
-      <c r="AJ6">
+      <c r="AI6">
+        <v>4158</v>
+      </c>
+      <c r="AL6">
         <v>10164</v>
       </c>
-      <c r="AK6">
+      <c r="AM6">
         <v>10048</v>
       </c>
-      <c r="AL6">
+      <c r="AN6">
         <v>10097</v>
       </c>
-      <c r="AM6">
+      <c r="AO6">
         <v>10096</v>
       </c>
-      <c r="AN6">
+      <c r="AP6">
         <v>10239</v>
       </c>
-      <c r="AO6">
+      <c r="AQ6">
         <v>10680</v>
       </c>
-      <c r="AP6">
+      <c r="AR6">
         <v>10755</v>
       </c>
-      <c r="AQ6">
+      <c r="AS6">
+        <v>11155</v>
+      </c>
+      <c r="AT6">
         <v>17725165</v>
       </c>
-      <c r="AR6">
+      <c r="AU6">
         <v>5924869</v>
       </c>
-      <c r="AS6">
+      <c r="AV6">
         <v>2014</v>
       </c>
-      <c r="AT6">
+      <c r="AW6">
         <v>2013</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AX6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AV6">
+      <c r="AY6">
+        <v>2016</v>
+      </c>
+      <c r="AZ6">
         <v>2015</v>
       </c>
-      <c r="AW6">
-        <v>2015</v>
-      </c>
-      <c r="AX6" t="s">
+      <c r="BA6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY6">
-        <v>2015</v>
-      </c>
-      <c r="AZ6" t="s">
+      <c r="BB6">
+        <v>2016</v>
+      </c>
+      <c r="BC6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA6">
-        <v>2015</v>
+      <c r="BD6">
+        <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>8610</v>
@@ -1395,106 +1465,115 @@
       <c r="J7">
         <v>9822</v>
       </c>
-      <c r="P7">
+      <c r="K7">
+        <v>9663</v>
+      </c>
+      <c r="Q7">
         <v>9370</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>9680</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>9916</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>10154</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>10312</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>10624</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>10819</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>5936</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>6066</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>5938</v>
       </c>
-      <c r="AD7">
-        <v>5845</v>
-      </c>
       <c r="AE7">
+        <v>5848</v>
+      </c>
+      <c r="AF7">
         <v>5593</v>
       </c>
-      <c r="AF7">
-        <v>4723</v>
-      </c>
       <c r="AG7">
-        <v>4804</v>
-      </c>
-      <c r="AJ7">
+        <v>4725</v>
+      </c>
+      <c r="AH7">
+        <v>4808</v>
+      </c>
+      <c r="AI7">
+        <v>5228</v>
+      </c>
+      <c r="AL7">
         <v>8011</v>
       </c>
-      <c r="AK7">
+      <c r="AM7">
         <v>7963</v>
       </c>
-      <c r="AL7">
+      <c r="AN7">
         <v>7958</v>
       </c>
-      <c r="AM7">
+      <c r="AO7">
         <v>7915</v>
       </c>
-      <c r="AN7">
+      <c r="AP7">
         <v>7892</v>
       </c>
-      <c r="AO7">
+      <c r="AQ7">
         <v>8250</v>
       </c>
-      <c r="AP7">
+      <c r="AR7">
         <v>8337</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7">
+        <v>8525</v>
+      </c>
+      <c r="AT7">
         <v>2463092</v>
       </c>
-      <c r="AR7">
+      <c r="AU7">
         <v>8000000</v>
       </c>
-      <c r="AS7">
+      <c r="AV7">
         <v>2013</v>
       </c>
-      <c r="AT7">
+      <c r="AW7">
         <v>2012</v>
       </c>
-      <c r="AU7" t="s">
+      <c r="AX7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AV7">
+      <c r="AY7">
+        <v>2016</v>
+      </c>
+      <c r="AZ7">
         <v>2015</v>
       </c>
-      <c r="AW7">
-        <v>2015</v>
-      </c>
-      <c r="AX7" t="s">
+      <c r="BA7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY7">
-        <v>2015</v>
-      </c>
-      <c r="AZ7" t="s">
+      <c r="BB7">
+        <v>2016</v>
+      </c>
+      <c r="BC7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA7">
-        <v>2015</v>
+      <c r="BD7">
+        <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8">
         <v>20625</v>
@@ -1520,100 +1599,109 @@
       <c r="J8">
         <v>21479</v>
       </c>
-      <c r="N8">
+      <c r="K8">
+        <v>23130</v>
+      </c>
+      <c r="O8">
         <v>20117</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>20900</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>21037</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>21174</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>21311</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>21448</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>21584</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>10091</v>
       </c>
-      <c r="AC8">
+      <c r="AD8">
         <v>10656</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>10338</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>12228</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>11659</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>11588</v>
       </c>
-      <c r="AK8">
+      <c r="AI8">
+        <v>10217</v>
+      </c>
+      <c r="AM8">
         <v>23269</v>
       </c>
-      <c r="AL8">
+      <c r="AN8">
         <v>23121</v>
       </c>
-      <c r="AM8">
+      <c r="AO8">
         <v>22658</v>
       </c>
-      <c r="AN8">
+      <c r="AP8">
         <v>22459</v>
       </c>
-      <c r="AO8">
+      <c r="AQ8">
         <v>22771</v>
       </c>
-      <c r="AP8">
+      <c r="AR8">
         <v>22314</v>
       </c>
-      <c r="AQ8">
+      <c r="AS8">
+        <v>22666</v>
+      </c>
+      <c r="AT8">
         <v>55700000</v>
       </c>
-      <c r="AR8">
+      <c r="AU8">
         <v>69617700</v>
       </c>
-      <c r="AS8">
+      <c r="AV8">
         <v>2011</v>
       </c>
-      <c r="AT8">
+      <c r="AW8">
         <v>2010</v>
       </c>
-      <c r="AU8" t="s">
+      <c r="AX8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY8">
+        <v>2016</v>
+      </c>
+      <c r="AZ8">
+        <v>2015</v>
+      </c>
+      <c r="BA8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB8">
+        <v>2016</v>
+      </c>
+      <c r="BC8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD8">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>63</v>
-      </c>
-      <c r="AV8">
-        <v>2015</v>
-      </c>
-      <c r="AW8">
-        <v>2015</v>
-      </c>
-      <c r="AX8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AY8">
-        <v>2015</v>
-      </c>
-      <c r="AZ8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="BA8">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>64</v>
       </c>
       <c r="C9">
         <v>38228</v>
@@ -1639,100 +1727,109 @@
       <c r="J9">
         <v>36377</v>
       </c>
-      <c r="O9">
+      <c r="K9">
+        <v>35682</v>
+      </c>
+      <c r="P9">
         <v>39311</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>39247</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>39178</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>39235</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>39335</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>23819</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <v>23607</v>
       </c>
-      <c r="AC9">
+      <c r="AD9">
         <v>26105</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>26494</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>27092</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <v>29619</v>
       </c>
-      <c r="AG9">
+      <c r="AH9">
         <v>31293</v>
       </c>
-      <c r="AJ9">
+      <c r="AI9">
+        <v>31176</v>
+      </c>
+      <c r="AL9">
         <v>40831</v>
       </c>
-      <c r="AK9">
+      <c r="AM9">
         <v>42834</v>
       </c>
-      <c r="AL9">
+      <c r="AN9">
         <v>43825</v>
       </c>
-      <c r="AM9">
+      <c r="AO9">
         <v>42866</v>
       </c>
-      <c r="AN9">
+      <c r="AP9">
         <v>42753</v>
       </c>
-      <c r="AO9">
+      <c r="AQ9">
         <v>40979</v>
       </c>
-      <c r="AP9">
+      <c r="AR9">
         <v>40883</v>
       </c>
-      <c r="AQ9">
+      <c r="AS9">
+        <v>39826</v>
+      </c>
+      <c r="AT9">
         <v>17249098</v>
       </c>
-      <c r="AR9">
+      <c r="AU9">
         <v>1700000</v>
       </c>
-      <c r="AS9">
+      <c r="AV9">
         <v>2011</v>
       </c>
-      <c r="AT9">
+      <c r="AW9">
         <v>2010</v>
       </c>
-      <c r="AU9" t="s">
+      <c r="AX9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY9">
+        <v>2016</v>
+      </c>
+      <c r="AZ9">
+        <v>2015</v>
+      </c>
+      <c r="BA9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB9">
+        <v>2016</v>
+      </c>
+      <c r="BC9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD9">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>65</v>
-      </c>
-      <c r="AV9">
-        <v>2015</v>
-      </c>
-      <c r="AW9">
-        <v>2015</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AY9">
-        <v>2015</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA9">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>66</v>
       </c>
       <c r="F10">
         <v>21367</v>
@@ -1749,97 +1846,106 @@
       <c r="J10">
         <v>18789</v>
       </c>
-      <c r="Q10">
+      <c r="K10">
+        <v>19531</v>
+      </c>
+      <c r="R10">
         <v>22497</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>22869</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>23230</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>23500</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>23611</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>23780</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>23903</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>23984</v>
       </c>
-      <c r="AC10">
+      <c r="AD10">
         <v>6829</v>
       </c>
-      <c r="AD10">
+      <c r="AE10">
         <v>6949</v>
       </c>
-      <c r="AE10">
+      <c r="AF10">
         <v>6483</v>
       </c>
-      <c r="AF10">
+      <c r="AG10">
         <v>8057</v>
       </c>
-      <c r="AG10">
+      <c r="AH10">
         <v>9692</v>
       </c>
-      <c r="AL10">
+      <c r="AI10">
+        <v>7679</v>
+      </c>
+      <c r="AN10">
         <v>27235</v>
       </c>
-      <c r="AM10">
+      <c r="AO10">
         <v>28293</v>
       </c>
-      <c r="AN10">
+      <c r="AP10">
         <v>29936</v>
       </c>
-      <c r="AO10">
+      <c r="AQ10">
         <v>30881</v>
       </c>
-      <c r="AP10">
+      <c r="AR10">
         <v>35145</v>
       </c>
-      <c r="AQ10">
+      <c r="AS10">
+        <v>28756</v>
+      </c>
+      <c r="AT10">
         <v>0</v>
       </c>
-      <c r="AR10">
+      <c r="AU10">
         <v>10850000</v>
       </c>
-      <c r="AS10">
+      <c r="AV10">
         <v>2014</v>
       </c>
-      <c r="AT10">
+      <c r="AW10">
         <v>2013</v>
       </c>
-      <c r="AU10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV10">
+      <c r="AX10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AY10">
+        <v>2016</v>
+      </c>
+      <c r="AZ10">
         <v>2015</v>
       </c>
-      <c r="AW10">
-        <v>2015</v>
-      </c>
-      <c r="AX10" t="s">
+      <c r="BA10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB10">
+        <v>2016</v>
+      </c>
+      <c r="BC10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD10">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>67</v>
-      </c>
-      <c r="AY10">
-        <v>2015</v>
-      </c>
-      <c r="AZ10" t="s">
-        <v>67</v>
-      </c>
-      <c r="BA10">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>68</v>
       </c>
       <c r="C11">
         <v>30415</v>
@@ -1865,106 +1971,115 @@
       <c r="J11">
         <v>32330</v>
       </c>
-      <c r="N11">
+      <c r="K11">
+        <v>32461</v>
+      </c>
+      <c r="O11">
         <v>30729</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>30739</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>30748</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>30758</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>30768</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>30777</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>30787</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>17558</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <v>17774</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>17703</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>17833</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>16888</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>16172</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>15109</v>
       </c>
-      <c r="AJ11">
+      <c r="AI11">
+        <v>14749</v>
+      </c>
+      <c r="AL11">
         <v>52742</v>
       </c>
-      <c r="AK11">
+      <c r="AM11">
         <v>53140</v>
       </c>
-      <c r="AL11">
+      <c r="AN11">
         <v>52635</v>
       </c>
-      <c r="AM11">
+      <c r="AO11">
         <v>53021</v>
       </c>
-      <c r="AN11">
+      <c r="AP11">
         <v>49798</v>
       </c>
-      <c r="AO11">
+      <c r="AQ11">
         <v>45867</v>
       </c>
-      <c r="AP11">
+      <c r="AR11">
         <v>42623</v>
       </c>
-      <c r="AQ11">
+      <c r="AS11">
+        <v>41159</v>
+      </c>
+      <c r="AT11">
         <v>0</v>
       </c>
-      <c r="AR11">
+      <c r="AU11">
         <v>0</v>
       </c>
-      <c r="AS11">
+      <c r="AV11">
         <v>2012</v>
       </c>
-      <c r="AT11">
+      <c r="AW11">
         <v>2011</v>
       </c>
-      <c r="AU11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AV11">
+      <c r="AX11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY11">
+        <v>2016</v>
+      </c>
+      <c r="AZ11">
         <v>2015</v>
       </c>
-      <c r="AW11">
-        <v>2015</v>
-      </c>
-      <c r="AX11" t="s">
+      <c r="BA11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY11">
-        <v>2015</v>
-      </c>
-      <c r="AZ11" t="s">
+      <c r="BB11">
+        <v>2016</v>
+      </c>
+      <c r="BC11" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA11">
-        <v>2015</v>
+      <c r="BD11">
+        <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>2778</v>
@@ -1987,106 +2102,115 @@
       <c r="J12">
         <v>2837</v>
       </c>
-      <c r="M12">
+      <c r="K12">
+        <v>2717</v>
+      </c>
+      <c r="N12">
         <v>2917</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>2878</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>2923</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>2960</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2989</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>3012</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>3029</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>1803</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <v>1869</v>
       </c>
-      <c r="AC12">
+      <c r="AD12">
         <v>2156</v>
       </c>
-      <c r="AD12">
+      <c r="AE12">
         <v>1885</v>
       </c>
-      <c r="AE12">
+      <c r="AF12">
         <v>1942</v>
       </c>
-      <c r="AF12">
+      <c r="AG12">
         <v>2185</v>
       </c>
-      <c r="AG12">
+      <c r="AH12">
         <v>2320</v>
       </c>
-      <c r="AJ12">
+      <c r="AI12">
+        <v>2390</v>
+      </c>
+      <c r="AL12">
         <v>4562</v>
       </c>
-      <c r="AK12">
+      <c r="AM12">
         <v>4502</v>
       </c>
-      <c r="AL12">
+      <c r="AN12">
         <v>4215</v>
       </c>
-      <c r="AM12">
+      <c r="AO12">
         <v>3803</v>
       </c>
-      <c r="AN12">
+      <c r="AP12">
         <v>3896</v>
       </c>
-      <c r="AO12">
+      <c r="AQ12">
         <v>3765</v>
       </c>
-      <c r="AP12">
+      <c r="AR12">
         <v>3692</v>
       </c>
-      <c r="AQ12">
+      <c r="AS12">
+        <v>3748</v>
+      </c>
+      <c r="AT12">
         <v>0</v>
       </c>
-      <c r="AR12">
+      <c r="AU12">
         <v>0</v>
       </c>
-      <c r="AS12">
+      <c r="AV12">
         <v>2010</v>
       </c>
-      <c r="AT12">
+      <c r="AW12">
         <v>2009</v>
       </c>
-      <c r="AU12" t="s">
+      <c r="AX12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AV12">
+      <c r="AY12">
+        <v>2016</v>
+      </c>
+      <c r="AZ12">
         <v>2015</v>
       </c>
-      <c r="AW12">
-        <v>2015</v>
-      </c>
-      <c r="AX12" t="s">
+      <c r="BA12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY12">
-        <v>2015</v>
-      </c>
-      <c r="AZ12" t="s">
+      <c r="BB12">
+        <v>2016</v>
+      </c>
+      <c r="BC12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA12">
-        <v>2015</v>
+      <c r="BD12">
+        <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13">
         <v>39326</v>
@@ -2112,115 +2236,124 @@
       <c r="J13">
         <v>37794</v>
       </c>
-      <c r="O13">
+      <c r="K13">
+        <v>37440</v>
+      </c>
+      <c r="P13">
         <v>41811</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>41987</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>42013</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>42267</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>42562</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>42898</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>43220</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>43664</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>44208</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>44840</v>
-      </c>
-      <c r="AA13">
-        <v>4329</v>
       </c>
       <c r="AB13">
         <v>4329</v>
       </c>
       <c r="AC13">
+        <v>4329</v>
+      </c>
+      <c r="AD13">
         <v>4258</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>4622</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>6582</v>
       </c>
-      <c r="AF13">
+      <c r="AG13">
         <v>9380</v>
       </c>
-      <c r="AG13">
+      <c r="AH13">
         <v>11762</v>
       </c>
-      <c r="AJ13">
+      <c r="AI13">
+        <v>13332</v>
+      </c>
+      <c r="AL13">
         <v>109540</v>
       </c>
-      <c r="AK13">
+      <c r="AM13">
         <v>107414</v>
       </c>
-      <c r="AL13">
+      <c r="AN13">
         <v>103882</v>
       </c>
-      <c r="AM13">
+      <c r="AO13">
         <v>103163</v>
       </c>
-      <c r="AN13">
+      <c r="AP13">
         <v>98436</v>
       </c>
-      <c r="AO13">
+      <c r="AQ13">
         <v>94020</v>
       </c>
-      <c r="AP13">
+      <c r="AR13">
         <v>89106</v>
       </c>
-      <c r="AQ13">
+      <c r="AS13">
+        <v>85212</v>
+      </c>
+      <c r="AT13">
         <v>164678859</v>
       </c>
-      <c r="AR13">
+      <c r="AU13">
         <v>30308962</v>
       </c>
-      <c r="AS13">
+      <c r="AV13">
         <v>2011</v>
       </c>
-      <c r="AT13">
+      <c r="AW13">
         <v>2010</v>
       </c>
-      <c r="AU13" t="s">
+      <c r="AX13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AV13">
+      <c r="AY13">
+        <v>2016</v>
+      </c>
+      <c r="AZ13">
         <v>2015</v>
       </c>
-      <c r="AW13">
-        <v>2015</v>
-      </c>
-      <c r="AX13" t="s">
+      <c r="BA13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY13">
-        <v>2015</v>
-      </c>
-      <c r="AZ13" t="s">
+      <c r="BB13">
+        <v>2016</v>
+      </c>
+      <c r="BC13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA13">
-        <v>2015</v>
+      <c r="BD13">
+        <v>2016</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14">
         <v>50884</v>
@@ -2246,103 +2379,112 @@
       <c r="J14">
         <v>50651</v>
       </c>
-      <c r="N14">
+      <c r="K14">
+        <v>50556</v>
+      </c>
+      <c r="O14">
         <v>50987</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>51297</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>52164</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>52784</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>53413</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>53858</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>13637</v>
       </c>
-      <c r="AB14">
+      <c r="AC14">
         <v>10774</v>
       </c>
-      <c r="AC14">
+      <c r="AD14">
         <v>11729</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <v>13944</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <v>16088</v>
       </c>
-      <c r="AF14">
+      <c r="AG14">
         <v>16633</v>
       </c>
-      <c r="AG14">
+      <c r="AH14">
         <v>17541</v>
       </c>
-      <c r="AJ14">
+      <c r="AI14">
+        <v>18884</v>
+      </c>
+      <c r="AL14">
         <v>14927</v>
       </c>
-      <c r="AK14">
+      <c r="AM14">
         <v>11500</v>
       </c>
-      <c r="AL14">
+      <c r="AN14">
         <v>11985</v>
       </c>
-      <c r="AM14">
+      <c r="AO14">
         <v>12137</v>
       </c>
-      <c r="AN14">
+      <c r="AP14">
         <v>12642</v>
       </c>
-      <c r="AO14">
+      <c r="AQ14">
         <v>12248</v>
       </c>
-      <c r="AP14">
+      <c r="AR14">
         <v>12418</v>
       </c>
-      <c r="AQ14">
+      <c r="AS14">
+        <v>12156</v>
+      </c>
+      <c r="AT14">
         <v>0</v>
       </c>
-      <c r="AR14">
+      <c r="AU14">
         <v>22600000</v>
       </c>
-      <c r="AS14">
+      <c r="AV14">
         <v>2011</v>
       </c>
-      <c r="AT14">
+      <c r="AW14">
         <v>2010</v>
       </c>
-      <c r="AU14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AV14">
+      <c r="AX14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY14">
+        <v>2016</v>
+      </c>
+      <c r="AZ14">
         <v>2015</v>
       </c>
-      <c r="AW14">
-        <v>2015</v>
-      </c>
-      <c r="AX14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AY14">
-        <v>2015</v>
-      </c>
-      <c r="AZ14" t="s">
-        <v>65</v>
-      </c>
-      <c r="BA14">
-        <v>2015</v>
+      <c r="BA14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB14">
+        <v>2016</v>
+      </c>
+      <c r="BC14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD14">
+        <v>2016</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15">
         <v>25200</v>
@@ -2365,85 +2507,85 @@
       <c r="J15">
         <v>28871</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>3706</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <v>3538</v>
       </c>
-      <c r="AC15">
+      <c r="AD15">
         <v>3300</v>
       </c>
-      <c r="AD15">
+      <c r="AE15">
         <v>3069</v>
       </c>
-      <c r="AE15">
+      <c r="AF15">
         <v>3059</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>3204</v>
       </c>
-      <c r="AG15">
+      <c r="AH15">
         <v>2981</v>
       </c>
-      <c r="AJ15">
+      <c r="AL15">
         <v>27464</v>
       </c>
-      <c r="AK15">
+      <c r="AM15">
         <v>24711</v>
       </c>
-      <c r="AL15">
+      <c r="AN15">
         <v>21629</v>
       </c>
-      <c r="AM15">
+      <c r="AO15">
         <v>20815</v>
       </c>
-      <c r="AN15">
+      <c r="AP15">
         <v>21085</v>
       </c>
-      <c r="AO15">
+      <c r="AQ15">
         <v>21586</v>
       </c>
-      <c r="AP15">
+      <c r="AR15">
         <v>22957</v>
       </c>
-      <c r="AQ15">
+      <c r="AT15">
         <v>0</v>
       </c>
-      <c r="AR15">
+      <c r="AU15">
         <v>6933539</v>
       </c>
-      <c r="AS15">
+      <c r="AV15">
         <v>2012</v>
       </c>
-      <c r="AT15">
+      <c r="AW15">
         <v>2011</v>
       </c>
-      <c r="AU15" t="s">
+      <c r="AX15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AY15">
+        <v>2016</v>
+      </c>
+      <c r="AZ15">
+        <v>2015</v>
+      </c>
+      <c r="BA15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB15">
+        <v>2016</v>
+      </c>
+      <c r="BC15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD15">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>73</v>
-      </c>
-      <c r="AV15">
-        <v>2015</v>
-      </c>
-      <c r="AW15">
-        <v>2015</v>
-      </c>
-      <c r="AX15" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY15">
-        <v>2015</v>
-      </c>
-      <c r="AZ15" t="s">
-        <v>73</v>
-      </c>
-      <c r="BA15">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>74</v>
       </c>
       <c r="E16">
         <v>13924</v>
@@ -2463,97 +2605,106 @@
       <c r="J16">
         <v>14655</v>
       </c>
-      <c r="Q16">
+      <c r="K16">
+        <v>14617</v>
+      </c>
+      <c r="R16">
         <v>14635</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>14823</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>14981</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>15158</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>15338</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>15498</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <v>13382</v>
       </c>
-      <c r="AC16">
+      <c r="AD16">
         <v>13358</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>13422</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>13628</v>
       </c>
-      <c r="AF16">
+      <c r="AG16">
         <v>14105</v>
       </c>
-      <c r="AG16">
+      <c r="AH16">
         <v>14041</v>
       </c>
-      <c r="AK16">
+      <c r="AI16">
+        <v>14122</v>
+      </c>
+      <c r="AM16">
         <v>17423</v>
       </c>
-      <c r="AL16">
+      <c r="AN16">
         <v>17605</v>
       </c>
-      <c r="AM16">
+      <c r="AO16">
         <v>17377</v>
       </c>
-      <c r="AN16">
+      <c r="AP16">
         <v>17385</v>
       </c>
-      <c r="AO16">
+      <c r="AQ16">
         <v>17697</v>
       </c>
-      <c r="AP16">
+      <c r="AR16">
         <v>17184</v>
       </c>
-      <c r="AQ16">
+      <c r="AS16">
+        <v>16299</v>
+      </c>
+      <c r="AT16">
         <v>18408538</v>
       </c>
-      <c r="AR16">
+      <c r="AU16">
         <v>98000000</v>
       </c>
-      <c r="AS16">
+      <c r="AV16">
         <v>2013</v>
       </c>
-      <c r="AT16">
+      <c r="AW16">
         <v>2012</v>
       </c>
-      <c r="AU16" t="s">
+      <c r="AX16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY16">
+        <v>2016</v>
+      </c>
+      <c r="AZ16">
+        <v>2015</v>
+      </c>
+      <c r="BA16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="BB16">
+        <v>2016</v>
+      </c>
+      <c r="BC16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD16">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="17" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>75</v>
-      </c>
-      <c r="AV16">
-        <v>2015</v>
-      </c>
-      <c r="AW16">
-        <v>2015</v>
-      </c>
-      <c r="AX16" t="s">
-        <v>75</v>
-      </c>
-      <c r="AY16">
-        <v>2015</v>
-      </c>
-      <c r="AZ16" t="s">
-        <v>75</v>
-      </c>
-      <c r="BA16">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="17" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>76</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -2578,115 +2729,124 @@
       <c r="J17" s="1">
         <v>50366</v>
       </c>
-      <c r="K17"/>
+      <c r="K17">
+        <v>49913</v>
+      </c>
       <c r="L17"/>
       <c r="M17"/>
       <c r="N17"/>
-      <c r="O17" s="1">
+      <c r="O17"/>
+      <c r="P17" s="1">
         <v>51638</v>
       </c>
-      <c r="P17" s="1">
+      <c r="Q17" s="1">
         <v>51722</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="R17" s="1">
         <v>52279</v>
       </c>
-      <c r="R17" s="1">
+      <c r="S17" s="1">
         <v>52236</v>
       </c>
-      <c r="S17" s="1">
+      <c r="T17" s="1">
         <v>51693</v>
       </c>
-      <c r="T17" s="1">
+      <c r="U17" s="1">
         <v>51151</v>
       </c>
-      <c r="U17"/>
       <c r="V17"/>
       <c r="W17"/>
       <c r="X17"/>
       <c r="Y17"/>
       <c r="Z17"/>
-      <c r="AA17">
+      <c r="AA17"/>
+      <c r="AB17">
         <v>23224</v>
       </c>
-      <c r="AB17">
+      <c r="AC17">
         <v>24633</v>
       </c>
-      <c r="AC17">
+      <c r="AD17">
         <v>26486</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>27913</v>
       </c>
-      <c r="AE17">
+      <c r="AF17">
         <v>30025</v>
       </c>
-      <c r="AF17">
+      <c r="AG17">
         <v>31726</v>
       </c>
-      <c r="AG17">
+      <c r="AH17">
         <v>33076</v>
       </c>
-      <c r="AH17"/>
-      <c r="AI17"/>
-      <c r="AJ17">
+      <c r="AI17">
+        <v>33129</v>
+      </c>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17">
         <v>7876</v>
       </c>
-      <c r="AK17">
+      <c r="AM17">
         <v>8140</v>
       </c>
-      <c r="AL17">
+      <c r="AN17">
         <v>8235</v>
       </c>
-      <c r="AM17">
+      <c r="AO17">
         <v>8324</v>
       </c>
-      <c r="AN17">
+      <c r="AP17">
         <v>8091</v>
       </c>
-      <c r="AO17">
+      <c r="AQ17">
         <v>8084</v>
       </c>
-      <c r="AP17">
+      <c r="AR17">
         <v>8193</v>
       </c>
-      <c r="AQ17">
+      <c r="AS17">
+        <v>8277</v>
+      </c>
+      <c r="AT17">
         <v>12858000</v>
       </c>
-      <c r="AR17">
+      <c r="AU17">
         <v>3986000</v>
       </c>
-      <c r="AS17">
+      <c r="AV17">
         <v>2012</v>
       </c>
-      <c r="AT17">
+      <c r="AW17">
         <v>2011</v>
       </c>
-      <c r="AU17" s="2" t="s">
+      <c r="AX17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AV17">
+      <c r="AY17">
+        <v>2016</v>
+      </c>
+      <c r="AZ17">
         <v>2015</v>
       </c>
-      <c r="AW17">
-        <v>2015</v>
-      </c>
-      <c r="AX17" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AY17">
-        <v>2015</v>
-      </c>
-      <c r="AZ17" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="BA17">
-        <v>2015</v>
+      <c r="BA17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB17">
+        <v>2016</v>
+      </c>
+      <c r="BC17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD17">
+        <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18">
         <v>24138</v>
@@ -2715,103 +2875,112 @@
       <c r="J18">
         <v>21773</v>
       </c>
-      <c r="M18">
+      <c r="K18">
+        <v>21308</v>
+      </c>
+      <c r="N18">
         <v>24612</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>25565</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>26082</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>26861</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>27810</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>27903</v>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <v>2950</v>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <v>3009</v>
       </c>
-      <c r="AC18">
+      <c r="AD18">
         <v>2853</v>
       </c>
-      <c r="AD18">
+      <c r="AE18">
         <v>2846</v>
       </c>
-      <c r="AE18">
+      <c r="AF18">
         <v>3033</v>
       </c>
-      <c r="AF18">
+      <c r="AG18">
         <v>3135</v>
       </c>
-      <c r="AG18">
+      <c r="AH18">
         <v>3532</v>
       </c>
-      <c r="AJ18">
+      <c r="AI18">
+        <v>3371</v>
+      </c>
+      <c r="AL18">
         <v>26694</v>
       </c>
-      <c r="AK18">
+      <c r="AM18">
         <v>26157</v>
       </c>
-      <c r="AL18">
+      <c r="AN18">
         <v>25902</v>
       </c>
-      <c r="AM18">
+      <c r="AO18">
         <v>27824</v>
       </c>
-      <c r="AN18">
+      <c r="AP18">
         <v>29173</v>
       </c>
-      <c r="AO18">
+      <c r="AQ18">
         <v>28021</v>
       </c>
-      <c r="AP18">
+      <c r="AR18">
         <v>26809</v>
       </c>
-      <c r="AQ18">
+      <c r="AS18">
+        <v>25132</v>
+      </c>
+      <c r="AT18">
         <v>491000000</v>
       </c>
-      <c r="AR18">
+      <c r="AU18">
         <v>0</v>
       </c>
-      <c r="AS18">
+      <c r="AV18">
         <v>2010</v>
       </c>
-      <c r="AT18">
+      <c r="AW18">
         <v>2009</v>
       </c>
-      <c r="AU18" t="s">
-        <v>82</v>
-      </c>
-      <c r="AV18">
-        <v>2015</v>
-      </c>
-      <c r="AW18">
+      <c r="AX18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AY18">
+        <v>2016</v>
+      </c>
+      <c r="AZ18">
         <v>2014</v>
       </c>
-      <c r="AX18" t="s">
+      <c r="BA18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY18">
-        <v>2015</v>
-      </c>
-      <c r="AZ18" t="s">
+      <c r="BB18">
+        <v>2016</v>
+      </c>
+      <c r="BC18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA18">
-        <v>2015</v>
+      <c r="BD18">
+        <v>2016</v>
       </c>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19">
         <v>3450</v>
@@ -2831,103 +3000,115 @@
       <c r="J19">
         <v>3588</v>
       </c>
-      <c r="P19">
+      <c r="K19">
+        <v>3586</v>
+      </c>
+      <c r="Q19">
         <v>3636</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>3717</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>3833</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>3942</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>4070</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>4213</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>4336</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>2749</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>2787</v>
       </c>
-      <c r="AC19">
+      <c r="AD19">
         <v>2884</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>2800</v>
       </c>
-      <c r="AE19">
+      <c r="AF19">
         <v>2910</v>
       </c>
-      <c r="AF19">
+      <c r="AG19">
         <v>2630</v>
       </c>
-      <c r="AG19">
+      <c r="AH19">
         <v>2627</v>
       </c>
-      <c r="AK19">
+      <c r="AI19">
+        <v>2671</v>
+      </c>
+      <c r="AL19">
+        <v>3241</v>
+      </c>
+      <c r="AM19">
         <v>3326</v>
       </c>
-      <c r="AL19">
+      <c r="AN19">
         <v>3682</v>
       </c>
-      <c r="AM19">
+      <c r="AO19">
         <v>4325</v>
       </c>
-      <c r="AN19">
+      <c r="AP19">
         <v>5011</v>
       </c>
-      <c r="AO19">
-        <v>5415</v>
-      </c>
-      <c r="AP19">
-        <v>5918</v>
-      </c>
       <c r="AQ19">
+        <v>5474</v>
+      </c>
+      <c r="AR19">
+        <v>5977</v>
+      </c>
+      <c r="AS19">
+        <v>6032</v>
+      </c>
+      <c r="AT19">
         <v>41328334</v>
       </c>
-      <c r="AR19">
+      <c r="AU19">
         <v>9464854</v>
       </c>
-      <c r="AS19">
+      <c r="AV19">
         <v>2013</v>
       </c>
-      <c r="AT19">
+      <c r="AW19">
         <v>2012</v>
       </c>
-      <c r="AU19" t="s">
-        <v>79</v>
-      </c>
-      <c r="AV19">
+      <c r="AX19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY19">
+        <v>2016</v>
+      </c>
+      <c r="AZ19">
         <v>2015</v>
       </c>
-      <c r="AW19">
-        <v>2015</v>
-      </c>
-      <c r="AX19" t="s">
+      <c r="BA19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AY19">
-        <v>2015</v>
-      </c>
-      <c r="AZ19" t="s">
+      <c r="BB19">
+        <v>2016</v>
+      </c>
+      <c r="BC19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA19">
-        <v>2015</v>
+      <c r="BD19">
+        <v>2016</v>
       </c>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20">
         <v>6367</v>
@@ -2948,76 +3129,82 @@
         <v>6896</v>
       </c>
       <c r="J20">
-        <v>6965</v>
-      </c>
-      <c r="P20">
+        <v>7118</v>
+      </c>
+      <c r="K20">
+        <v>7053</v>
+      </c>
+      <c r="Q20">
         <v>7146</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>7531</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>7821</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>8072</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>8304</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>8633</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>8893</v>
       </c>
-      <c r="AA20">
+      <c r="AB20">
         <v>1491</v>
       </c>
-      <c r="AB20">
+      <c r="AC20">
         <v>1264</v>
       </c>
-      <c r="AC20">
+      <c r="AD20">
         <v>1466</v>
       </c>
-      <c r="AD20">
+      <c r="AE20">
         <v>1498</v>
       </c>
-      <c r="AE20">
+      <c r="AF20">
         <v>1813</v>
       </c>
-      <c r="AF20">
+      <c r="AG20">
         <v>2074</v>
       </c>
-      <c r="AG20">
+      <c r="AH20">
         <v>2088</v>
       </c>
-      <c r="AQ20">
+      <c r="AI20">
+        <v>2014</v>
+      </c>
+      <c r="AT20">
         <v>24895115</v>
       </c>
-      <c r="AR20">
+      <c r="AU20">
         <v>11600000</v>
       </c>
-      <c r="AS20">
+      <c r="AV20">
         <v>2013</v>
       </c>
-      <c r="AT20">
+      <c r="AW20">
         <v>2012</v>
       </c>
-      <c r="AU20" t="s">
+      <c r="AX20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AV20">
+      <c r="AY20">
+        <v>2016</v>
+      </c>
+      <c r="AZ20">
         <v>2015</v>
       </c>
-      <c r="AW20">
-        <v>2015</v>
-      </c>
-      <c r="AZ20" t="s">
+      <c r="BC20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BA20">
-        <v>2015</v>
+      <c r="BD20">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add recent update year and change update language
</commit_message>
<xml_diff>
--- a/data/source/JRI infographic data.xlsx
+++ b/data/source/JRI infographic data.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/jri/data/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\JWelshlo\Documents\JRI\data tracker\Text and Data for Comms\June 2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="760" windowWidth="21400" windowHeight="19880"/>
+    <workbookView xWindow="12195" yWindow="45" windowWidth="12015" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -302,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -643,27 +637,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="25" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10" customWidth="1"/>
-    <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="36" width="9.140625" customWidth="1"/>
+    <col min="37" max="37" width="10" customWidth="1"/>
+    <col min="38" max="43" width="9.140625" customWidth="1"/>
+    <col min="44" max="45" width="10" customWidth="1"/>
+    <col min="46" max="46" width="11" customWidth="1"/>
+    <col min="47" max="47" width="11.85546875" customWidth="1"/>
+    <col min="48" max="49" width="9.140625" customWidth="1"/>
+    <col min="50" max="50" width="19.5703125" style="3" customWidth="1"/>
+    <col min="51" max="51" width="9.140625" customWidth="1"/>
+    <col min="52" max="52" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="17" style="3" customWidth="1"/>
-    <col min="54" max="54" width="11.5" customWidth="1"/>
-    <col min="55" max="55" width="17.83203125" style="3" customWidth="1"/>
+    <col min="54" max="54" width="11.42578125" customWidth="1"/>
+    <col min="55" max="55" width="17.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:56" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +831,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -958,7 +956,7 @@
         <v>2016</v>
       </c>
       <c r="AZ2">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA2" s="3" t="s">
         <v>54</v>
@@ -973,7 +971,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1056,7 +1054,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1166,7 +1164,7 @@
         <v>2016</v>
       </c>
       <c r="AZ4">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA4" s="3" t="s">
         <v>88</v>
@@ -1181,7 +1179,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -1294,7 +1292,7 @@
         <v>2016</v>
       </c>
       <c r="AZ5">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA5" s="3" t="s">
         <v>54</v>
@@ -1309,7 +1307,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1425,7 +1423,7 @@
         <v>2016</v>
       </c>
       <c r="AZ6">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA6" s="3" t="s">
         <v>54</v>
@@ -1440,7 +1438,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -1556,7 +1554,7 @@
         <v>2016</v>
       </c>
       <c r="AZ7">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA7" s="3" t="s">
         <v>54</v>
@@ -1571,7 +1569,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1684,7 +1682,7 @@
         <v>2016</v>
       </c>
       <c r="AZ8">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA8" s="3" t="s">
         <v>76</v>
@@ -1699,7 +1697,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1827,7 +1825,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1928,7 +1926,7 @@
         <v>2016</v>
       </c>
       <c r="AZ10">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA10" s="3" t="s">
         <v>66</v>
@@ -1943,7 +1941,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -2062,7 +2060,7 @@
         <v>2016</v>
       </c>
       <c r="AZ11">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA11" s="3" t="s">
         <v>54</v>
@@ -2077,7 +2075,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -2208,7 +2206,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -2336,7 +2334,7 @@
         <v>2016</v>
       </c>
       <c r="AZ13">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA13" s="3" t="s">
         <v>54</v>
@@ -2351,7 +2349,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -2482,7 +2480,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -2583,7 +2581,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2687,7 +2685,7 @@
         <v>2016</v>
       </c>
       <c r="AZ16">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA16" s="3" t="s">
         <v>74</v>
@@ -2702,7 +2700,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="17" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -2829,7 +2827,7 @@
         <v>2016</v>
       </c>
       <c r="AZ17">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA17" s="3" t="s">
         <v>84</v>
@@ -2844,7 +2842,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -2978,7 +2976,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -3091,7 +3089,7 @@
         <v>2016</v>
       </c>
       <c r="AZ19">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BA19" s="3" t="s">
         <v>54</v>
@@ -3106,7 +3104,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -3198,7 +3196,7 @@
         <v>2016</v>
       </c>
       <c r="AZ20">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="BC20" s="3" t="s">
         <v>54</v>

</xml_diff>